<commit_message>
new models and adjusted cross-validation
</commit_message>
<xml_diff>
--- a/figures_and_tables/table_appendix_hyperparameters_CS.xlsx
+++ b/figures_and_tables/table_appendix_hyperparameters_CS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,140 +463,280 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CatBoost</t>
+          <t>AdaBoost</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>learning_rate: 0.03
-l2_leaf_reg: 4
-iterations: 150
-depth: 6</t>
+          <t>n_estimators: 100
+learning_rate: 0.1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>learning_rate: 0.03
-l2_leaf_reg: 4
-iterations: 150
-depth: 6</t>
+          <t>n_estimators: 200
+learning_rate: 1.0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>learning_rate: 0.03
-l2_leaf_reg: 0.5
-iterations: 150
-depth: 2</t>
+          <t>n_estimators: 200
+learning_rate: 1.0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>learning_rate: 0.03
-l2_leaf_reg: 0.5
-iterations: 150
-depth: 2</t>
+          <t>n_estimators: 200
+learning_rate: 1.0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>BaggedDT</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>n_estimators: 100
+base_estimator__max_depth: 5</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>n_estimators: 100
+base_estimator__max_depth: 5</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>n_estimators: 100
+base_estimator__max_depth: 10</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>n_estimators: 100
+base_estimator__max_depth: 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BayesianNN</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>n_iter: 100
+lambda_2: 0.0001
+lambda_1: 1e-06
+alpha_2: 1e-06
+alpha_1: 0.0001</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>n_iter: 300
+lambda_2: 0.0001
+lambda_1: 0.0001
+alpha_2: 1e-06
+alpha_1: 0.0001</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>n_iter: 100
+lambda_2: 0.0001
+lambda_1: 1e-06
+alpha_2: 1e-06
+alpha_1: 0.0001</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>n_iter: 100
+lambda_2: 0.0001
+lambda_1: 1e-06
+alpha_2: 1e-06
+alpha_1: 0.0001</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CatBoost</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>learning_rate: 0.1
+l2_leaf_reg: 3
+iterations: 100
+depth: 2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>learning_rate: 0.1
+l2_leaf_reg: 3
+iterations: 100
+depth: 2</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>learning_rate: 0.03
+l2_leaf_reg: 1
+iterations: 250
+depth: 4</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>learning_rate: 0.1
+l2_leaf_reg: 0.2
+iterations: 200
+depth: 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>GBDT</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>subsample: 1
+n_estimators: 50
+max_leaf_nodes: 100
+max_depth: 2
+learning_rate: 0.1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>subsample: 1
+n_estimators: 50
+max_leaf_nodes: 100
+max_depth: 2
+learning_rate: 0.1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>subsample: 0.5
-n_estimators: 100
-max_leaf_nodes: 20
-max_depth: 4
-learning_rate: 0.01</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>subsample: 0.5
-n_estimators: 100
-max_leaf_nodes: 20
-max_depth: 4
-learning_rate: 0.01</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>subsample: 1
-n_estimators: 1000
+n_estimators: 200
 max_leaf_nodes: 100
 max_depth: 4
 learning_rate: 0.01</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>subsample: 1
-n_estimators: 1000
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>subsample: 0.5
+n_estimators: 200
 max_leaf_nodes: 100
 max_depth: 4
 learning_rate: 0.01</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>KNN</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>n_neighbors: 17</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>n_neighbors: 21</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>n_neighbors: 17</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>n_neighbors: 21</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>n_neighbors: 8</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>n_neighbors: 10</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>n_neighbors: 9</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>n_neighbors: 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LightGBM</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>n_estimators: 50
+max_depth: 4
+learning_rate: 0.05</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>n_estimators: 50
+max_depth: 10
+learning_rate: 0.05</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>n_estimators: 50
+max_depth: 4
+learning_rate: 0.1</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>n_estimators: 50
+max_depth: 10
+learning_rate: 0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>MLP</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>max_iter: 20
+learning_rate_init: 0.01
+hidden_layer_sizes: [64]</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t>max_iter: 50
 learning_rate_init: 0.01
-hidden_layer_sizes: [8]</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>max_iter: 50
+hidden_layer_sizes: [64]</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>max_iter: 20
 learning_rate_init: 0.01
-hidden_layer_sizes: [8]</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>max_iter: 50
-learning_rate_init: 0.01
-hidden_layer_sizes: [8]</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
+hidden_layer_sizes: [128]</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>max_iter: 50
 learning_rate_init: 0.01
@@ -604,112 +744,139 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>RF</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>n_estimators: 1200
-min_samples_split: 16
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>n_estimators: 600
+min_samples_split: 10
 min_samples_leaf: 5
-max_features: 5
-max_depth: 120</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>n_estimators: 400
-min_samples_split: 16
-min_samples_leaf: 4
-max_features: 4
-max_depth: 150</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>n_estimators: 1000
+max_features: 6
+max_depth: 100</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>n_estimators: 200
 min_samples_split: 10
 min_samples_leaf: 5
 max_features: 6
 max_depth: 150</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>n_estimators: 1200
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>n_estimators: 600
+min_samples_split: 12
+min_samples_leaf: 4
+max_features: 6
+max_depth: 140</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>n_estimators: 600
 min_samples_split: 10
-min_samples_leaf: 6
+min_samples_leaf: 5
 max_features: 6
-max_depth: 120</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+max_depth: 100</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
         <is>
           <t>SVR</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>gamma: 1e-05
 C: 10</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>gamma: 1e-05
 C: 10</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>gamma: 1e-05
-C: 1000</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
+C: 100</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>gamma: 1e-05
-C: 10</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+C: 100</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>StackEns</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>final_estimator__alpha: 10.0</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>final_estimator__alpha: 10.0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>final_estimator__alpha: 0.1</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>final_estimator__alpha: 0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
         <is>
           <t>XGBoost</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>n_estimators: 800
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>n_estimators: 500
 max_depth: 4
 learning_rate: 0.015</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>n_estimators: 500
+max_depth: 4
+learning_rate: 0.02</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>n_estimators: 500
+max_depth: 5
+learning_rate: 0.02</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>n_estimators: 700
 max_depth: 4
-learning_rate: 0.01</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>n_estimators: 500
-max_depth: 5
 learning_rate: 0.015</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>n_estimators: 700
-max_depth: 4
-learning_rate: 0.01</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update with spatial clustering
</commit_message>
<xml_diff>
--- a/figures_and_tables/table_appendix_hyperparameters_CS.xlsx
+++ b/figures_and_tables/table_appendix_hyperparameters_CS.xlsx
@@ -478,7 +478,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>50</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -510,12 +510,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>0.1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1.0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -542,22 +542,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>100</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>50</t>
         </is>
       </c>
     </row>
@@ -574,12 +574,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -589,7 +589,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>100</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -675,7 +675,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>1e-06</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -766,17 +766,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>0.1</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>0.1</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>0.03</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -798,17 +798,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -830,12 +830,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>250</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>250</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -862,17 +862,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>2</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>4</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -926,22 +926,22 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>2000</t>
         </is>
       </c>
     </row>
@@ -958,22 +958,22 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>20</t>
         </is>
       </c>
     </row>
@@ -995,17 +995,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1022,22 +1022,22 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>0.1</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>0.1</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>0.01</t>
         </is>
       </c>
     </row>
@@ -1054,22 +1054,22 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1086,22 +1086,22 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>50</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>100</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>100</t>
         </is>
       </c>
     </row>
@@ -1118,22 +1118,22 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -1155,17 +1155,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
           <t>0.05</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>0.1</t>
-        </is>
-      </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0.1</t>
+          <t>0.05</t>
         </is>
       </c>
     </row>
@@ -1182,17 +1182,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>50</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
           <t>50</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>20</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1224,12 +1224,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0.01</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>0.01</t>
+          <t>0.1</t>
         </is>
       </c>
     </row>
@@ -1246,22 +1246,22 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>[8]</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>[8]</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
           <t>[64]</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>[64]</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>[128]</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>[4]</t>
         </is>
       </c>
     </row>
@@ -1283,12 +1283,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
           <t>200</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>600</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1315,12 +1315,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
           <t>10</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>12</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1347,17 +1347,17 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>4</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>5</t>
         </is>
       </c>
     </row>
@@ -1411,17 +1411,17 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
           <t>150</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>140</t>
-        </is>
-      </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>120</t>
         </is>
       </c>
     </row>
@@ -1470,17 +1470,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>100</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>100</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1534,22 +1534,22 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>600</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>600</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>600</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>800</t>
         </is>
       </c>
     </row>
@@ -1566,17 +1566,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>4</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>5</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1608,7 +1608,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0.02</t>
+          <t>0.01</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">

</xml_diff>

<commit_message>
update with DeepCNN code and results
</commit_message>
<xml_diff>
--- a/figures_and_tables/table_appendix_hyperparameters_CS.xlsx
+++ b/figures_and_tables/table_appendix_hyperparameters_CS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -884,34 +884,14 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GBDT</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>subsample</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
+          <t>DeepCNN</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -921,27 +901,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>n_estimators</t>
+          <t>subsample</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>0.5</t>
         </is>
       </c>
     </row>
@@ -953,27 +933,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>max_leaf_nodes</t>
+          <t>n_estimators</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>2000</t>
         </is>
       </c>
     </row>
@@ -985,27 +965,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>max_depth</t>
+          <t>max_leaf_nodes</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>20</t>
         </is>
       </c>
     </row>
@@ -1017,91 +997,91 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>learning_rate</t>
+          <t>max_depth</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.01</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.01</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>0.1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>KNN</t>
+          <t>GBDT</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>n_neighbors</t>
+          <t>learning_rate</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0.01</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0.01</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0.1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LightGBM</t>
+          <t>KNN</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>n_estimators</t>
+          <t>n_neighbors</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1113,27 +1093,27 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>max_depth</t>
+          <t>n_estimators</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>100</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>50</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>100</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>100</t>
         </is>
       </c>
     </row>
@@ -1145,59 +1125,59 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>learning_rate</t>
+          <t>max_depth</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.05</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.05</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0.05</t>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>MLP</t>
+          <t>LightGBM</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>max_iter</t>
+          <t>learning_rate</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>0.05</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>0.05</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>0.05</t>
         </is>
       </c>
     </row>
@@ -1209,27 +1189,27 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>learning_rate_init</t>
+          <t>max_iter</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.01</t>
+          <t>50</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.01</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0.1</t>
+          <t>50</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>0.1</t>
+          <t>50</t>
         </is>
       </c>
     </row>
@@ -1241,59 +1221,59 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>hidden_layer_sizes</t>
+          <t>learning_rate_init</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>0.01</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>0.01</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>[64]</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>[64]</t>
+          <t>0.1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>RF</t>
+          <t>MLP</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>n_estimators</t>
+          <t>hidden_layer_sizes</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>[8]</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>[8]</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>[64]</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>[64]</t>
         </is>
       </c>
     </row>
@@ -1305,27 +1285,27 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>min_samples_split</t>
+          <t>n_estimators</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>600</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>400</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>200</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>600</t>
         </is>
       </c>
     </row>
@@ -1337,27 +1317,27 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>min_samples_leaf</t>
+          <t>min_samples_split</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>10</t>
         </is>
       </c>
     </row>
@@ -1369,27 +1349,27 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>max_features</t>
+          <t>min_samples_leaf</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1401,59 +1381,59 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>max_depth</t>
+          <t>max_features</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>6</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>SVR</t>
+          <t>RF</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>gamma</t>
+          <t>max_depth</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1e-05</t>
+          <t>100</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1e-05</t>
+          <t>120</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1e-05</t>
+          <t>150</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>1e-05</t>
+          <t>120</t>
         </is>
       </c>
     </row>
@@ -1465,91 +1445,91 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>gamma</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>1e-05</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>1e-05</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1e-05</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>1e-05</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>StackEns</t>
+          <t>SVR</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>final_estimator__alpha</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.1</t>
+          <t>100</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>100</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.1</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>0.1</t>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>XGBoost</t>
+          <t>StackEns</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>n_estimators</t>
+          <t>final_estimator__alpha</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>800</t>
+          <t>0.1</t>
         </is>
       </c>
     </row>
@@ -1561,27 +1541,27 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>max_depth</t>
+          <t>n_estimators</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>600</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>600</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>600</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>800</t>
         </is>
       </c>
     </row>
@@ -1593,25 +1573,57 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>max_depth</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>XGBoost</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
           <t>learning_rate</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>0.015</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>0.02</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>0.01</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>0.015</t>
         </is>

</xml_diff>